<commit_message>
Updated the logic_BOM to have the SSR Board
</commit_message>
<xml_diff>
--- a/2015/Hardware/logic_BOM.xlsx
+++ b/2015/Hardware/logic_BOM.xlsx
@@ -1,14 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\minerfiles.mst.edu\dfs\users\ncv8cc\Desktop\GitHub\Battery-Management-System\2015\Hardware\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Logic" sheetId="1" r:id="rId1"/>
+    <sheet name="SSR" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="56">
   <si>
     <t>Quantity</t>
   </si>
@@ -115,16 +120,93 @@
   </si>
   <si>
     <t>102-1265-1-ND</t>
+  </si>
+  <si>
+    <t>acs770</t>
+  </si>
+  <si>
+    <t>High Power Terminal</t>
+  </si>
+  <si>
+    <t>current sense</t>
+  </si>
+  <si>
+    <t>D_STP5045S</t>
+  </si>
+  <si>
+    <t>Diode</t>
+  </si>
+  <si>
+    <t>Through hole</t>
+  </si>
+  <si>
+    <t>60k</t>
+  </si>
+  <si>
+    <t>Resistor</t>
+  </si>
+  <si>
+    <t>SPDT</t>
+  </si>
+  <si>
+    <t>Switch</t>
+  </si>
+  <si>
+    <t>PTSCMD</t>
+  </si>
+  <si>
+    <t>Poly-fuse</t>
+  </si>
+  <si>
+    <t>lt1910</t>
+  </si>
+  <si>
+    <t>Mosfet driver</t>
+  </si>
+  <si>
+    <t>SOIC-8</t>
+  </si>
+  <si>
+    <t>irls3034-7p</t>
+  </si>
+  <si>
+    <t>Mosfet</t>
+  </si>
+  <si>
+    <t>Surface mount</t>
+  </si>
+  <si>
+    <t>10uF</t>
+  </si>
+  <si>
+    <t>Capacitor</t>
+  </si>
+  <si>
+    <t>H3373-ND</t>
+  </si>
+  <si>
+    <t>Connector</t>
+  </si>
+  <si>
+    <t>FIND THE MALE CONNECTOR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -147,13 +229,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -161,6 +246,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -209,7 +297,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -244,7 +332,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -455,8 +543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -687,12 +775,194 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5">
+        <v>1206</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6">
+        <v>1206</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8">
+        <v>1206</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11">
+        <v>1206</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" t="s">
+        <v>50</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E12" r:id="rId1" display="http://www.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;itemSeq=165378352&amp;uq=635580674242796387&amp;CSRT=10282226202437667372"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
BOM adjustment i think
</commit_message>
<xml_diff>
--- a/2015/Hardware/logic_BOM.xlsx
+++ b/2015/Hardware/logic_BOM.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="22220" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Logic" sheetId="1" r:id="rId1"/>
     <sheet name="SSR" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -574,13 +579,13 @@
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="3" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -597,7 +602,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>1</v>
       </c>
@@ -605,7 +610,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>1</v>
       </c>
@@ -616,7 +621,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>1</v>
       </c>
@@ -630,7 +635,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8">
         <v>1</v>
       </c>
@@ -644,7 +649,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9">
         <v>1</v>
       </c>
@@ -658,7 +663,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10">
         <v>1</v>
       </c>
@@ -672,7 +677,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11">
         <v>1</v>
       </c>
@@ -686,7 +691,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12">
         <v>2</v>
       </c>
@@ -700,7 +705,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13">
         <v>3</v>
       </c>
@@ -714,7 +719,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14">
         <v>2</v>
       </c>
@@ -728,7 +733,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15">
         <v>2</v>
       </c>
@@ -742,7 +747,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16">
         <v>2</v>
       </c>
@@ -753,7 +758,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17">
         <v>3</v>
       </c>
@@ -767,7 +772,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18">
         <v>9</v>
       </c>
@@ -780,6 +785,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -788,19 +798,19 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -817,7 +827,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>1</v>
       </c>
@@ -834,7 +844,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>1</v>
       </c>
@@ -854,7 +864,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>1</v>
       </c>
@@ -871,7 +881,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>1</v>
       </c>
@@ -888,7 +898,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>1</v>
       </c>
@@ -905,7 +915,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>1</v>
       </c>
@@ -922,7 +932,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>1</v>
       </c>
@@ -939,7 +949,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9">
         <v>1</v>
       </c>
@@ -956,7 +966,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10">
         <v>1</v>
       </c>
@@ -973,7 +983,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11">
         <v>1</v>
       </c>
@@ -990,7 +1000,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1012,6 +1022,12 @@
     <hyperlink ref="E12" r:id="rId1" display="http://www.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;itemSeq=165378352&amp;uq=635580674242796387&amp;CSRT=10282226202437667372"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1021,8 +1037,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>